<commit_message>
Add save model function
</commit_message>
<xml_diff>
--- a/data/results/model_results_nn.xlsx
+++ b/data/results/model_results_nn.xlsx
@@ -538,23 +538,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 100, 'model__learning_rate': 0.01, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 2, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-76.21358177387468</v>
+        <v>-172.8527694896686</v>
       </c>
       <c r="E2" t="n">
-        <v>-263.0689163294657</v>
+        <v>-261.2691374453992</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.229002550601206</v>
+        <v>-0.1555368039808629</v>
       </c>
       <c r="G2" t="n">
-        <v>16.6447508363174</v>
+        <v>15.72131944615002</v>
       </c>
       <c r="H2" t="n">
-        <v>678.7692482200724</v>
+        <v>691.3090721403909</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>73.94924235343933</v>
+        <v>144.8301923274994</v>
       </c>
     </row>
     <row r="3">
@@ -616,23 +616,23 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 200, 'model__learning_rate': 0.01, 'model__hidden_size': 50}</t>
+          <t>{'model__num_layers': 2, 'model__num_epochs': 1000, 'model__learning_rate': 0.01, 'model__hidden_size': 50}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-160.7580232544244</v>
+        <v>-76.6727051768876</v>
       </c>
       <c r="E3" t="n">
-        <v>-226.8895753783898</v>
+        <v>-242.2800866981888</v>
       </c>
       <c r="F3" t="n">
-        <v>0.01608986630485353</v>
+        <v>-1.37409088851563</v>
       </c>
       <c r="G3" t="n">
-        <v>15.03586814989238</v>
+        <v>24.9399623209483</v>
       </c>
       <c r="H3" t="n">
-        <v>608.1032876890587</v>
+        <v>1170.379548839687</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>32.64133310317993</v>
+        <v>158.2019264698029</v>
       </c>
     </row>
     <row r="4">
@@ -694,23 +694,23 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 2, 'model__num_epochs': 200, 'model__learning_rate': 0.001, 'model__hidden_size': 50}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-142.6497586821358</v>
+        <v>-196.1482591672423</v>
       </c>
       <c r="E4" t="n">
-        <v>-255.129899818783</v>
+        <v>-298.8487153428299</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.009093469703249349</v>
+        <v>0.002907464150800033</v>
       </c>
       <c r="G4" t="n">
-        <v>14.88500105910105</v>
+        <v>15.05971658410547</v>
       </c>
       <c r="H4" t="n">
-        <v>645.4507290429571</v>
+        <v>628.0208864998216</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>20.89496493339539</v>
+        <v>151.3259847164154</v>
       </c>
     </row>
     <row r="5">
@@ -776,19 +776,19 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-160.8824764232333</v>
+        <v>-161.7739497669316</v>
       </c>
       <c r="E5" t="n">
-        <v>-224.9075076568167</v>
+        <v>-227.0103812347398</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.01317673015982396</v>
+        <v>-0.01199033354670448</v>
       </c>
       <c r="G5" t="n">
-        <v>14.91068937197124</v>
+        <v>14.97530084975778</v>
       </c>
       <c r="H5" t="n">
-        <v>631.3448607820079</v>
+        <v>627.1710922436423</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="R5" t="n">
-        <v>31.48666882514954</v>
+        <v>81.75265431404114</v>
       </c>
     </row>
     <row r="6">
@@ -850,23 +850,23 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 2, 'model__num_epochs': 200, 'model__learning_rate': 0.01, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 2, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-35.4948269605226</v>
+        <v>-152.0897618055957</v>
       </c>
       <c r="E6" t="n">
-        <v>-261.8600848407647</v>
+        <v>-252.3588980430893</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.4187413732671086</v>
+        <v>-0.07467443601760616</v>
       </c>
       <c r="G6" t="n">
-        <v>18.344313742415</v>
+        <v>15.20127800723733</v>
       </c>
       <c r="H6" t="n">
-        <v>753.9131710412288</v>
+        <v>659.409719107261</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>7.82252049446106</v>
+        <v>74.70702195167542</v>
       </c>
     </row>
     <row r="7">
@@ -928,23 +928,23 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 200, 'model__learning_rate': 0.01, 'model__hidden_size': 50}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 200, 'model__learning_rate': 0.01, 'model__hidden_size': 100}</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-161.4605619812797</v>
+        <v>-135.7946958025966</v>
       </c>
       <c r="E7" t="n">
-        <v>-228.0672724240043</v>
+        <v>-212.0371116356648</v>
       </c>
       <c r="F7" t="n">
-        <v>0.03316205524977636</v>
+        <v>-0.1371438836669445</v>
       </c>
       <c r="G7" t="n">
-        <v>14.93063921318751</v>
+        <v>16.86700426136522</v>
       </c>
       <c r="H7" t="n">
-        <v>596.3643889341782</v>
+        <v>649.4439889931624</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -990,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>8.085662364959717</v>
+        <v>67.73950147628784</v>
       </c>
     </row>
     <row r="8">
@@ -1006,23 +1006,23 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 2, 'model__num_epochs': 200, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 200, 'model__learning_rate': 0.001, 'model__hidden_size': 50}</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-108.3504860361824</v>
+        <v>-135.7096714671342</v>
       </c>
       <c r="E8" t="n">
-        <v>-261.2287887600744</v>
+        <v>-282.0976000018738</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.3237724610919255</v>
+        <v>-0.0616693587328205</v>
       </c>
       <c r="G8" t="n">
-        <v>17.83794996387882</v>
+        <v>15.32435088053141</v>
       </c>
       <c r="H8" t="n">
-        <v>697.4319932927623</v>
+        <v>641.645778393803</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -1068,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="n">
-        <v>8.602067232131958</v>
+        <v>127.9376130104065</v>
       </c>
     </row>
     <row r="9">
@@ -1084,23 +1084,23 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 100, 'model__learning_rate': 0.01, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 100, 'model__learning_rate': 0.01, 'model__hidden_size': 50}</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-156.2295383943183</v>
+        <v>-170.3885490090783</v>
       </c>
       <c r="E9" t="n">
-        <v>-218.8570680506928</v>
+        <v>-229.3575651894215</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.008395149232483065</v>
+        <v>-0.02148651825069288</v>
       </c>
       <c r="G9" t="n">
-        <v>14.91909325691119</v>
+        <v>14.98958668103501</v>
       </c>
       <c r="H9" t="n">
-        <v>629.9151329006576</v>
+        <v>647.2581252329063</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>7.906118869781494</v>
+        <v>76.35982370376587</v>
       </c>
     </row>
     <row r="10">
@@ -1166,19 +1166,19 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-129.6639090065599</v>
+        <v>-130.1377172414571</v>
       </c>
       <c r="E10" t="n">
-        <v>-257.409741130339</v>
+        <v>-259.9469519184787</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.01917343487534867</v>
+        <v>-0.02723020329831707</v>
       </c>
       <c r="G10" t="n">
-        <v>15.11764344711826</v>
+        <v>15.09695897312469</v>
       </c>
       <c r="H10" t="n">
-        <v>623.3838454193225</v>
+        <v>625.1326716294051</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1224,7 +1224,7 @@
         <v>0</v>
       </c>
       <c r="R10" t="n">
-        <v>6.681602001190186</v>
+        <v>8.293279647827148</v>
       </c>
     </row>
     <row r="11">
@@ -1244,19 +1244,19 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-168.6725824197462</v>
+        <v>-171.4621561722359</v>
       </c>
       <c r="E11" t="n">
-        <v>-235.2745240789166</v>
+        <v>-245.6482793673779</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.03439440478666286</v>
+        <v>-0.03677607512387978</v>
       </c>
       <c r="G11" t="n">
-        <v>15.442797931166</v>
+        <v>15.50050531474423</v>
       </c>
       <c r="H11" t="n">
-        <v>640.1873932984164</v>
+        <v>636.0944931596936</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="R11" t="n">
-        <v>7.405017375946045</v>
+        <v>38.15863180160522</v>
       </c>
     </row>
     <row r="12">
@@ -1318,23 +1318,23 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 200, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 2, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-113.8748046655068</v>
+        <v>-165.6760429019877</v>
       </c>
       <c r="E12" t="n">
-        <v>-229.8420819962926</v>
+        <v>-237.7659667535859</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.06215905606710694</v>
+        <v>-0.02446209747770381</v>
       </c>
       <c r="G12" t="n">
-        <v>15.74147177149716</v>
+        <v>15.11521404488446</v>
       </c>
       <c r="H12" t="n">
-        <v>611.7390881574595</v>
+        <v>657.4556169624924</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="R12" t="n">
-        <v>7.682931661605835</v>
+        <v>57.44451189041138</v>
       </c>
     </row>
     <row r="13">
@@ -1400,19 +1400,19 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-178.5373527091898</v>
+        <v>-178.9240506885007</v>
       </c>
       <c r="E13" t="n">
-        <v>-221.2130494773691</v>
+        <v>-221.0614181646161</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.03952139613890014</v>
+        <v>-0.03471829223772793</v>
       </c>
       <c r="G13" t="n">
-        <v>15.1678289860242</v>
+        <v>15.10966319262709</v>
       </c>
       <c r="H13" t="n">
-        <v>659.2700937228182</v>
+        <v>655.9333324449693</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="R13" t="n">
-        <v>8.140232086181641</v>
+        <v>50.47422766685486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add threading to pipeline
</commit_message>
<xml_diff>
--- a/data/results/model_results_nn.xlsx
+++ b/data/results/model_results_nn.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:BM13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,57 +471,292 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>MSE</t>
+          <t>X_Features</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>X_Features</t>
+          <t>Y_Target</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Y_Target</t>
+          <t>Start_date</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Start_date</t>
+          <t>End_date</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>End_date</t>
+          <t>Predict_start_date</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Predict_start_date</t>
+          <t>Predict_end_date</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Predict_end_date</t>
+          <t>Lookback</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Lookback</t>
+          <t>Horizon</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Horizon</t>
+          <t>Mode</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Mode</t>
+          <t>Duration (seconds)</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Duration (seconds)</t>
+          <t>MAE_T_0</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_1</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_2</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_3</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_4</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_5</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_6</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_7</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_8</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_9</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_10</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_11</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_12</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_13</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_14</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_15</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_16</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_17</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_18</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_19</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_20</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_21</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_22</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>MAE_T_23</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_0</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_1</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_2</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_3</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_4</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_5</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_6</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_7</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_8</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_9</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_10</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_11</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_12</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_13</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_14</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_15</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_16</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_17</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_18</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_19</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_20</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_21</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_22</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>R2_T_23</t>
         </is>
       </c>
     </row>
@@ -538,69 +773,210 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 2, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 17}</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-172.8527694896686</v>
+        <v>-95.14029944926375</v>
       </c>
       <c r="E2" t="n">
-        <v>-261.2691374453992</v>
+        <v>-404.4765327814765</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.1555368039808629</v>
+        <v>-0.05755358554458989</v>
       </c>
       <c r="G2" t="n">
-        <v>15.72131944615002</v>
-      </c>
-      <c r="H2" t="n">
-        <v>691.3090721403909</v>
+        <v>14.07755251397835</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>324.8580293655396</v>
       </c>
       <c r="R2" t="n">
-        <v>144.8301923274994</v>
+        <v>9.616535204770553</v>
+      </c>
+      <c r="S2" t="n">
+        <v>9.580582217599856</v>
+      </c>
+      <c r="T2" t="n">
+        <v>9.631320937009901</v>
+      </c>
+      <c r="U2" t="n">
+        <v>9.738348236346139</v>
+      </c>
+      <c r="V2" t="n">
+        <v>10.13348574186786</v>
+      </c>
+      <c r="W2" t="n">
+        <v>10.86715417739845</v>
+      </c>
+      <c r="X2" t="n">
+        <v>11.7395790761565</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>13.09597203872179</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>14.9297485260182</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>16.38596646841379</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>15.82901487254952</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>15.77261228488528</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>16.06889056562976</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>16.09764331453389</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>14.19219954795822</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>13.52852853041002</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>14.94982017467946</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>18.56820845186543</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>23.96204105681846</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>22.42493161261066</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>16.72090399315384</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>12.80454350884803</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>10.71312099414726</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>10.51010880308749</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.3078777975664949</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.3081601173741413</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.301141225192692</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.2934557223459063</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.2628364140996792</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.1860421480028963</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.1063038734481948</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>-0.02287753574149654</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>-0.1287453508426117</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>-0.169711938465519</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>-0.1450062621651453</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>-0.2065235404077113</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>-0.2571679089342243</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>-0.1751412934836452</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>-0.1077160975532154</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>-0.1360360798761078</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>-0.2875695994825551</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>-0.2325142438561931</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>-0.1219150547833319</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>-0.196001476623987</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>-0.3253309510847162</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>-0.3366408155614236</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>-0.1335179811797671</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>-0.1646872210585117</v>
       </c>
     </row>
     <row r="3">
@@ -616,69 +992,210 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 2, 'model__num_epochs': 1000, 'model__learning_rate': 0.01, 'model__hidden_size': 50}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 1}</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-76.6727051768876</v>
+        <v>-256.2832647401235</v>
       </c>
       <c r="E3" t="n">
-        <v>-242.2800866981888</v>
+        <v>-311.5768509199366</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.37409088851563</v>
+        <v>0.2098776350457039</v>
       </c>
       <c r="G3" t="n">
-        <v>24.9399623209483</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1170.379548839687</v>
+        <v>11.32935495401536</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>192.2861902713776</v>
       </c>
       <c r="R3" t="n">
-        <v>158.2019264698029</v>
+        <v>9.028453013503357</v>
+      </c>
+      <c r="S3" t="n">
+        <v>9.02572931469016</v>
+      </c>
+      <c r="T3" t="n">
+        <v>9.437135213060371</v>
+      </c>
+      <c r="U3" t="n">
+        <v>9.607527972509075</v>
+      </c>
+      <c r="V3" t="n">
+        <v>9.799596443152899</v>
+      </c>
+      <c r="W3" t="n">
+        <v>10.26555976269475</v>
+      </c>
+      <c r="X3" t="n">
+        <v>10.57184218856789</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>10.92129480140534</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>11.72067536493975</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>12.32952935472053</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>11.95689419663154</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>11.23110428486192</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>11.39576918795063</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>11.82251791553586</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>10.67149867532446</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>9.981250320130799</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>10.60847569985266</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>13.4537804625717</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>19.06511812078643</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>17.74751954745518</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>13.37175755821801</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>9.853191806179819</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>9.190674973924532</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>8.847622717701089</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.356119066734553</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.3108850930545779</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0.2560120061575343</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0.2163517663328632</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.196558030427908</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.1889472823121445</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0.1935527278789831</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0.2159997115431923</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0.2608336842893884</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0.2633596740167966</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0.3122013230658587</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>0.3049002513335607</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>0.2679570404058137</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>0.2568555580880225</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0.2846418348006833</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0.2958059477915778</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0.2506166705677835</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0.1233872002744592</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.01127680167148537</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0.02689060627883044</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.02215903518641815</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.1759139168801608</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0.1514157716036374</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0.0944222404006605</v>
       </c>
     </row>
     <row r="4">
@@ -694,69 +1211,210 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 2, 'model__num_epochs': 5000, 'model__learning_rate': 0.01, 'model__hidden_size': 1}</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-196.1482591672423</v>
+        <v>-167.934494268199</v>
       </c>
       <c r="E4" t="n">
-        <v>-298.8487153428299</v>
+        <v>-454.3095253462058</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002907464150800033</v>
+        <v>-0.1746927757389619</v>
       </c>
       <c r="G4" t="n">
-        <v>15.05971658410547</v>
-      </c>
-      <c r="H4" t="n">
-        <v>628.0208864998216</v>
+        <v>14.51036598975717</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>204.2647233009338</v>
       </c>
       <c r="R4" t="n">
-        <v>151.3259847164154</v>
+        <v>12.05132999519203</v>
+      </c>
+      <c r="S4" t="n">
+        <v>12.19545661152084</v>
+      </c>
+      <c r="T4" t="n">
+        <v>12.65395802488773</v>
+      </c>
+      <c r="U4" t="n">
+        <v>12.92052816592679</v>
+      </c>
+      <c r="V4" t="n">
+        <v>13.05005080676116</v>
+      </c>
+      <c r="W4" t="n">
+        <v>13.42190367470547</v>
+      </c>
+      <c r="X4" t="n">
+        <v>13.79033622098189</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>14.02924847620514</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>15.20329938233683</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>16.39876067490307</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>16.14930404301623</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>15.66472905860599</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>15.48661818904934</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>15.54516986103261</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>13.69352626755848</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>12.84079705551317</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>13.73736812711565</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>16.87689139621436</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>22.26447829343495</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>20.80192841143515</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>15.71176422989572</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>12.26483848634868</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>10.74662977213955</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>10.74986852939132</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>-0.08307657988691575</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>-0.1044968462952793</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>-0.1278446240870414</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>-0.1710617452377892</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>-0.1988512544612109</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>-0.2224535337143019</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>-0.2029545522850817</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>-0.1995654100318083</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>-0.2004870317715899</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>-0.2270802475054281</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>-0.2114638501991963</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>-0.2229388439324465</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>-0.2046848513183515</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>-0.1592361976163306</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>-0.1241114792139495</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>-0.1125605398673954</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>-0.1586236624631174</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>-0.1439400092040251</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>-0.09481725260446372</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>-0.135830998831957</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>-0.2295069919310697</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>-0.2644092436066976</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>-0.1783155849044609</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>-0.2143152867651767</v>
       </c>
     </row>
     <row r="5">
@@ -772,69 +1430,210 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 100, 'model__learning_rate': 0.01, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 26}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-161.7739497669316</v>
+        <v>-79.97536737098912</v>
       </c>
       <c r="E5" t="n">
-        <v>-227.0103812347398</v>
+        <v>-361.1377966552047</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.01199033354670448</v>
+        <v>0.07770930557007859</v>
       </c>
       <c r="G5" t="n">
-        <v>14.97530084975778</v>
-      </c>
-      <c r="H5" t="n">
-        <v>627.1710922436423</v>
+        <v>13.21147309459585</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>208.9859464168549</v>
       </c>
       <c r="R5" t="n">
-        <v>81.75265431404114</v>
+        <v>7.574294415013894</v>
+      </c>
+      <c r="S5" t="n">
+        <v>7.759367332101045</v>
+      </c>
+      <c r="T5" t="n">
+        <v>8.233331846085301</v>
+      </c>
+      <c r="U5" t="n">
+        <v>8.609119674658704</v>
+      </c>
+      <c r="V5" t="n">
+        <v>9.064972431650206</v>
+      </c>
+      <c r="W5" t="n">
+        <v>10.29591016687187</v>
+      </c>
+      <c r="X5" t="n">
+        <v>11.66798626229555</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>12.74720241176626</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>14.49451728640873</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>15.26573218308546</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>14.98820353164792</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>14.75463640197825</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>15.28933711030034</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>15.37411687124817</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>13.61925946378489</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>12.83976904958167</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>14.14793328707871</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>17.59849523812925</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>23.83759191536794</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>22.66152102491722</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>15.92333133168245</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>11.68163360093308</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>9.225846916444093</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>9.421244517269381</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.5649853354504492</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.5262678510558121</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>0.4752943320325153</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0.4184328584565633</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.3607848285890055</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.259456967246481</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.137408903579375</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>0.09119875660035648</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>-0.03014462326227862</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0.02180964733832635</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>0.01441940882265302</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>-0.03199250962063727</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>-0.1194890664050086</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>-0.06731902448412308</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>-0.03788796920063087</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>-0.03168177964525887</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>-0.1720063447501365</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>-0.1797083849974386</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>-0.09654188656868024</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>-0.1815419075128237</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>-0.170728084144935</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>-0.06918143642179997</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>0.1654361830121476</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0.01775127851195279</v>
       </c>
     </row>
     <row r="6">
@@ -850,69 +1649,210 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 2, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 74}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-152.0897618055957</v>
+        <v>-7.78253295517827</v>
       </c>
       <c r="E6" t="n">
-        <v>-252.3588980430893</v>
+        <v>-505.306950505451</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.07467443601760616</v>
+        <v>-0.1993334267499873</v>
       </c>
       <c r="G6" t="n">
-        <v>15.20127800723733</v>
-      </c>
-      <c r="H6" t="n">
-        <v>659.409719107261</v>
+        <v>15.2480811966636</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>160.6077330112457</v>
       </c>
       <c r="R6" t="n">
-        <v>74.70702195167542</v>
+        <v>8.748916592033501</v>
+      </c>
+      <c r="S6" t="n">
+        <v>8.987879725957169</v>
+      </c>
+      <c r="T6" t="n">
+        <v>10.00506965374691</v>
+      </c>
+      <c r="U6" t="n">
+        <v>10.71843701970649</v>
+      </c>
+      <c r="V6" t="n">
+        <v>11.43579431913949</v>
+      </c>
+      <c r="W6" t="n">
+        <v>12.67699398725267</v>
+      </c>
+      <c r="X6" t="n">
+        <v>14.03742259489523</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>14.84042751687793</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>15.76422618439661</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>17.25313228716271</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>16.78001349259081</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>17.30464159723672</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>18.18404474145676</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>18.64997829171536</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>15.48411967285304</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>14.01684122758767</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>15.50154327702341</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>19.58833471149106</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>26.28002252757544</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>24.23929960354548</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>17.54348428491357</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>13.76456264759461</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>11.56107547341153</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>12.58768728976227</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.4314598369531143</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.3877209949658119</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.2420124566130089</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0.143154358238216</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.02605153118109482</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>-0.1541420769033137</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>-0.3047821682096614</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>-0.3160211344226149</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>-0.2054800217230819</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>-0.2415576550214342</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>-0.2168653096150581</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>-0.3294692720043946</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>-0.4454165922762807</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>-0.3922927080509604</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>-0.2107570909017573</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>-0.1697612677092395</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>-0.3651070265439187</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>-0.3464947630946311</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>-0.2661150569698079</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>-0.3283476757205035</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>-0.3743362052782353</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>-0.4701984772266208</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>-0.2823669658071342</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>-0.5948899524722937</v>
       </c>
     </row>
     <row r="7">
@@ -928,69 +1868,210 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 200, 'model__learning_rate': 0.01, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 5}</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-135.7946958025966</v>
+        <v>-172.2828624239853</v>
       </c>
       <c r="E7" t="n">
-        <v>-212.0371116356648</v>
+        <v>-305.4464893989544</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1371438836669445</v>
+        <v>0.1836844285561527</v>
       </c>
       <c r="G7" t="n">
-        <v>16.86700426136522</v>
-      </c>
-      <c r="H7" t="n">
-        <v>649.4439889931624</v>
+        <v>11.90032383898827</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>182.5860936641693</v>
       </c>
       <c r="R7" t="n">
-        <v>67.73950147628784</v>
+        <v>9.446216975821102</v>
+      </c>
+      <c r="S7" t="n">
+        <v>9.301780635664324</v>
+      </c>
+      <c r="T7" t="n">
+        <v>9.631911239600656</v>
+      </c>
+      <c r="U7" t="n">
+        <v>9.993430914395434</v>
+      </c>
+      <c r="V7" t="n">
+        <v>10.2131507691972</v>
+      </c>
+      <c r="W7" t="n">
+        <v>10.72549011433764</v>
+      </c>
+      <c r="X7" t="n">
+        <v>11.12426661575224</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>11.35874258270964</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>12.51625468565165</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>13.3349089254055</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>12.74977591606012</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>12.27316995618976</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>12.3215814694555</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>12.62819434658127</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>10.89155131661617</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>10.19604256850471</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>10.86293258748778</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>13.66579251347492</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>18.97841276510567</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>18.27418915775179</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>13.88526757645426</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>11.41247699242163</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>9.907451334078507</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>9.914780177001017</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0.3287209002289543</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.3274519971828328</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0.280878409629376</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0.23752523194664</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.2189921572185936</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.1982899286903104</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>0.1913801290560302</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>0.1944156676411994</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>0.1719614242141392</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>0.1510768238213287</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>0.1974806631452417</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>0.1973763534144918</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0.1850464271859315</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>0.2146697549924782</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>0.2823357916512413</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>0.288428770631637</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0.2279863933324274</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>0.2280134315600192</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0.1928472264940569</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>0.134021986838635</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0.0440100674215318</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>-0.04097099380919889</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>0.02035270611659601</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>-0.06386496325682711</v>
       </c>
     </row>
     <row r="8">
@@ -1006,69 +2087,210 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 200, 'model__learning_rate': 0.001, 'model__hidden_size': 50}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 7}</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-135.7096714671342</v>
+        <v>-131.8467175489544</v>
       </c>
       <c r="E8" t="n">
-        <v>-282.0976000018738</v>
+        <v>-421.6805787370141</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.0616693587328205</v>
+        <v>-0.1342967567348136</v>
       </c>
       <c r="G8" t="n">
-        <v>15.32435088053141</v>
-      </c>
-      <c r="H8" t="n">
-        <v>641.645778393803</v>
+        <v>14.86085100973545</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>155.3720712661743</v>
       </c>
       <c r="R8" t="n">
-        <v>127.9376130104065</v>
+        <v>11.87623188337396</v>
+      </c>
+      <c r="S8" t="n">
+        <v>11.4330150170465</v>
+      </c>
+      <c r="T8" t="n">
+        <v>11.58759736586585</v>
+      </c>
+      <c r="U8" t="n">
+        <v>11.72098975710647</v>
+      </c>
+      <c r="V8" t="n">
+        <v>11.96485886217077</v>
+      </c>
+      <c r="W8" t="n">
+        <v>12.39368647872288</v>
+      </c>
+      <c r="X8" t="n">
+        <v>12.86666537318588</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>13.4782789224461</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>15.71611801044865</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>17.02541602975267</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>16.68962469436527</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>16.31456791636993</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>16.27413741779967</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>16.16215617723013</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>14.06970431149061</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>13.09825444618922</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>14.14444914661396</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>17.15991408766795</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>22.40792675865956</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>21.99146162881533</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>18.04633150258804</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>14.89599922176379</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>12.80587400185497</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>12.53716522212269</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>0.02922758391315716</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0.09743313576392953</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>0.08252749246939162</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>0.0587380869216011</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0.02870631023854187</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>-0.001291178801439585</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>-0.008485487963594052</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>-0.06513661340388199</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>-0.1694565028271073</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>-0.221942437676069</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>-0.1842686101344313</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>-0.1750185980033039</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>-0.1731282679968962</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>-0.0841255194068542</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>-0.03794277307263694</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>-0.03219882793538353</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>-0.1214350526172565</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>-0.0319353352399927</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>0.06484148722923488</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>-0.09673557974195957</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>-0.4031692206942126</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>-0.6671329926401881</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>-0.5520082500595906</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>-0.5591850099565852</v>
       </c>
     </row>
     <row r="9">
@@ -1084,69 +2306,210 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 100, 'model__learning_rate': 0.01, 'model__hidden_size': 50}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 82}</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-170.3885490090783</v>
+        <v>-31.22937686745314</v>
       </c>
       <c r="E9" t="n">
-        <v>-229.3575651894215</v>
+        <v>-415.3585608601185</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.02148651825069288</v>
+        <v>-0.0565423178554405</v>
       </c>
       <c r="G9" t="n">
-        <v>14.98958668103501</v>
-      </c>
-      <c r="H9" t="n">
-        <v>647.2581252329063</v>
+        <v>14.33633151316176</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>196.4914407730103</v>
       </c>
       <c r="R9" t="n">
-        <v>76.35982370376587</v>
+        <v>7.441013359295463</v>
+      </c>
+      <c r="S9" t="n">
+        <v>8.044062465812123</v>
+      </c>
+      <c r="T9" t="n">
+        <v>8.900785986642195</v>
+      </c>
+      <c r="U9" t="n">
+        <v>9.541153750440978</v>
+      </c>
+      <c r="V9" t="n">
+        <v>10.11489317586082</v>
+      </c>
+      <c r="W9" t="n">
+        <v>11.32682461751073</v>
+      </c>
+      <c r="X9" t="n">
+        <v>12.46305929189583</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>13.15339171732293</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>14.58516990566838</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>16.00075419848766</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>16.12878773310576</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>16.41746877121198</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>17.16712777638836</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>17.21457362292774</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>14.59929296927723</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>13.54191311678514</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>15.29269890529237</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>19.28832390346204</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>26.3874216628345</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>24.92102237666914</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>17.41497480099784</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>12.89998623524034</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>10.21172256244234</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>11.01553341031037</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>0.5707838795607807</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>0.491880865856885</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>0.384311494980329</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0.284125919332884</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.2129385115487704</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.0831281557348722</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.00608057600863221</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.003463462424645236</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>-0.03680990091532022</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>-0.06156519353441059</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>-0.09162149021402644</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>-0.1928301785957003</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>-0.3106779696719859</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>-0.2232798795544475</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>-0.1141437509681189</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>-0.0819986479058552</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>-0.2836889699209839</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>-0.2997858092626935</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>-0.266296189577909</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>-0.3584896654035783</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>-0.3527190933904019</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>-0.321318677223891</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>-0.05118143163618494</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>-0.3473216462028632</v>
       </c>
     </row>
     <row r="10">
@@ -1162,69 +2525,210 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 2, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 2, 'model__num_epochs': 5000, 'model__learning_rate': 0.01, 'model__hidden_size': 3}</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-130.1377172414571</v>
+        <v>-134.3511164674535</v>
       </c>
       <c r="E10" t="n">
-        <v>-259.9469519184787</v>
+        <v>-561.8119797302381</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.02723020329831707</v>
+        <v>-0.2168571073419407</v>
       </c>
       <c r="G10" t="n">
-        <v>15.09695897312469</v>
-      </c>
-      <c r="H10" t="n">
-        <v>625.1326716294051</v>
+        <v>15.17404915268442</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>92.05868577957153</v>
       </c>
       <c r="R10" t="n">
-        <v>8.293279647827148</v>
+        <v>11.39463887375748</v>
+      </c>
+      <c r="S10" t="n">
+        <v>11.37007720313065</v>
+      </c>
+      <c r="T10" t="n">
+        <v>11.65957523040421</v>
+      </c>
+      <c r="U10" t="n">
+        <v>11.90187268453717</v>
+      </c>
+      <c r="V10" t="n">
+        <v>12.28808665347136</v>
+      </c>
+      <c r="W10" t="n">
+        <v>12.67942633006693</v>
+      </c>
+      <c r="X10" t="n">
+        <v>13.35939165465938</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>13.98272759122979</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>15.45069761915045</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>17.15846869316802</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>17.30713747211183</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>16.79605675639312</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>16.81963565710786</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>17.31158532942091</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>15.09089218623862</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>14.03931122641068</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>14.63242854285277</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>18.3608855751353</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>26.05795379160374</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>24.00110565004965</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>17.14602640290432</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>13.248433825728</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>11.35266533158496</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>10.76809938330891</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>0.03939778688800477</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>0.0217457412570492</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>-0.02206046833905551</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>-0.06959849679554142</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>-0.1108498736647978</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>-0.1358824889376187</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>-0.1833695901475321</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>-0.1977436870662788</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>-0.203221834832499</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>-0.2227920429310977</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>-0.2466724007711552</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>-0.278871585185241</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>-0.2952262953966729</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>-0.2691513592701653</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>-0.205387327617949</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>-0.219533192707857</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>-0.3078857047358903</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>-0.3462913056085313</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>-0.3481101179789663</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>-0.3627060193862173</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>-0.3689386757388784</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>-0.3367216958748573</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>-0.2482103400246025</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>-0.2864896013402256</v>
       </c>
     </row>
     <row r="11">
@@ -1240,69 +2744,210 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 100, 'model__learning_rate': 0.01, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 15}</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-171.4621561722359</v>
+        <v>-149.3107410777961</v>
       </c>
       <c r="E11" t="n">
-        <v>-245.6482793673779</v>
+        <v>-306.5592404906786</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.03677607512387978</v>
+        <v>0.2004484853937514</v>
       </c>
       <c r="G11" t="n">
-        <v>15.50050531474423</v>
-      </c>
-      <c r="H11" t="n">
-        <v>636.0944931596936</v>
+        <v>11.88585588600515</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P11" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>102.0222661495209</v>
       </c>
       <c r="R11" t="n">
-        <v>38.15863180160522</v>
+        <v>9.072153278627576</v>
+      </c>
+      <c r="S11" t="n">
+        <v>8.979083264419533</v>
+      </c>
+      <c r="T11" t="n">
+        <v>9.305514000302617</v>
+      </c>
+      <c r="U11" t="n">
+        <v>9.82668382752251</v>
+      </c>
+      <c r="V11" t="n">
+        <v>10.22633153205553</v>
+      </c>
+      <c r="W11" t="n">
+        <v>10.81195808342515</v>
+      </c>
+      <c r="X11" t="n">
+        <v>11.18136342853317</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>11.52551316620854</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>12.66736308765849</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>13.76325311199264</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>13.03920358111045</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>12.72466803140334</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>12.73018337446624</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>12.96301184672637</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>11.17696789891358</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>10.25754800980527</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>10.87682686863851</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>13.40756674349728</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>18.76410146146019</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>18.14362465608141</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>13.78930275523025</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>10.93083952165636</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>9.478267568848228</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>9.619212165540416</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>0.3715440111510919</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0.3784177598223762</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>0.3363274952555971</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>0.2763877829371602</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.2414670438043701</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.2031373737165784</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>0.2007277199725898</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>0.2062716328238839</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>0.1789104882857186</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>0.1392933865214754</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>0.1793114389658917</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>0.1675600617391017</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>0.1688723480859453</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>0.1996072901669717</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>0.2612266945417996</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>0.2863987309209464</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>0.2283936811293964</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>0.2442727674397639</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>0.2029289513329678</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>0.1526126726412744</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>0.08823946918345871</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>0.04332240235711748</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>0.09075072099366555</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>-0.03521827433910807</v>
       </c>
     </row>
     <row r="12">
@@ -1318,69 +2963,210 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 2, 'model__num_epochs': 100, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 2, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 3}</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-165.6760429019877</v>
+        <v>-180.2919838021831</v>
       </c>
       <c r="E12" t="n">
-        <v>-237.7659667535859</v>
+        <v>-393.6752653059528</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.02446209747770381</v>
+        <v>0.08996979104582266</v>
       </c>
       <c r="G12" t="n">
-        <v>15.11521404488446</v>
-      </c>
-      <c r="H12" t="n">
-        <v>657.4556169624924</v>
+        <v>12.86541779857041</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>92.13471722602844</v>
       </c>
       <c r="R12" t="n">
-        <v>57.44451189041138</v>
+        <v>10.17750942850332</v>
+      </c>
+      <c r="S12" t="n">
+        <v>10.04964661534001</v>
+      </c>
+      <c r="T12" t="n">
+        <v>10.40739750886146</v>
+      </c>
+      <c r="U12" t="n">
+        <v>10.68650996292057</v>
+      </c>
+      <c r="V12" t="n">
+        <v>10.87453072667158</v>
+      </c>
+      <c r="W12" t="n">
+        <v>11.37174799048189</v>
+      </c>
+      <c r="X12" t="n">
+        <v>11.70707746424901</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>12.33836900817307</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>13.61040292143638</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>14.50428242698453</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>14.08483954296799</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>13.66391961396162</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>13.78201527769679</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>13.86209720951857</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>12.03878623913258</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>11.18240741528998</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>11.84343808816512</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>14.50064460387966</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>19.86965627686498</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>19.33093686608993</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>15.18124640344298</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>12.29451722359766</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>10.65493688424039</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>10.75311146721978</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>0.2376698508184865</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>0.2448494136017151</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>0.1982034558295462</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>0.1588104019099345</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.1325151496748149</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.1049368241797876</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.09583579074178417</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.07172335552213549</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.04534317110212904</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.04045001352734978</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.1114696952135223</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>0.1231179996404205</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>0.1135308797519713</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>0.1626181857980578</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>0.2027892198904192</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>0.2111266808775338</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>0.1410844658938557</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>0.1487507452923265</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>0.1555730700638999</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>0.08773661769541286</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>-0.06803496420273669</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>-0.2014592191582536</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>-0.1414501246885962</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>-0.2179156938757725</v>
       </c>
     </row>
     <row r="13">
@@ -1396,69 +3182,210 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'model__num_layers': 1, 'model__num_epochs': 200, 'model__learning_rate': 0.001, 'model__hidden_size': 100}</t>
+          <t>{'model__num_layers': 1, 'model__num_epochs': 5000, 'model__learning_rate': 0.001, 'model__hidden_size': 47}</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>-178.9240506885007</v>
+        <v>-64.20736354424393</v>
       </c>
       <c r="E13" t="n">
-        <v>-221.0614181646161</v>
+        <v>-414.3835555984848</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.03471829223772793</v>
+        <v>0.01591293676814699</v>
       </c>
       <c r="G13" t="n">
-        <v>15.10966319262709</v>
-      </c>
-      <c r="H13" t="n">
-        <v>655.9333324449693</v>
+        <v>14.06699122908269</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+        </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>['elec_prices_lag_1h', 'elec_prices_lag_2h', 'elec_prices_lag_3h', 'elec_prices_lag_4h', 'elec_prices_lag_5h', 'elec_prices_lag_6h', 'elec_prices_lag_7h', 'elec_prices_lag_8h', 'elec_prices_lag_9h', 'elec_prices_lag_10h', 'elec_prices_lag_11h', 'elec_prices_lag_12h', 'elec_prices_lag_13h', 'elec_prices_lag_14h', 'elec_prices_lag_15h', 'elec_prices_lag_16h', 'elec_prices_lag_17h', 'elec_prices_lag_18h', 'elec_prices_lag_19h', 'elec_prices_lag_20h', 'elec_prices_lag_21h', 'elec_prices_lag_22h', 'elec_prices_lag_23h', 'elec_prices_lag_24h', 'elec_prices_lag_25h', 'elec_prices_lag_26h', 'elec_prices_lag_27h', 'elec_prices_lag_28h', 'elec_prices_lag_29h', 'elec_prices_lag_30h', 'elec_prices_lag_31h', 'elec_prices_lag_32h', 'elec_prices_lag_33h', 'elec_prices_lag_34h', 'elec_prices_lag_35h', 'elec_prices_lag_36h', 'elec_prices_lag_37h', 'elec_prices_lag_38h', 'elec_prices_lag_39h', 'elec_prices_lag_40h', 'elec_prices_lag_41h', 'elec_prices_lag_42h', 'elec_prices_lag_43h', 'elec_prices_lag_44h', 'elec_prices_lag_45h', 'elec_prices_lag_46h', 'elec_prices_lag_47h', 'elec_prices_lag_48h', 'elec_prices_lag_49h', 'elec_prices_lag_50h', 'elec_prices_lag_51h', 'elec_prices_lag_52h', 'elec_prices_lag_53h', 'elec_prices_lag_54h', 'elec_prices_lag_55h', 'elec_prices_lag_56h', 'elec_prices_lag_57h', 'elec_prices_lag_58h', 'elec_prices_lag_59h', 'elec_prices_lag_60h', 'elec_prices_lag_61h', 'elec_prices_lag_62h', 'elec_prices_lag_63h', 'elec_prices_lag_64h', 'elec_prices_lag_65h', 'elec_prices_lag_66h', 'elec_prices_lag_67h', 'elec_prices_lag_68h', 'elec_prices_lag_69h', 'elec_prices_lag_70h', 'elec_prices_lag_71h', 'elec_prices_lag_72h', 'elec_prices_lag_73h', 'elec_prices_lag_74h', 'elec_prices_lag_75h', 'elec_prices_lag_76h', 'elec_prices_lag_77h', 'elec_prices_lag_78h', 'elec_prices_lag_79h', 'elec_prices_lag_80h', 'elec_prices_lag_81h', 'elec_prices_lag_82h', 'elec_prices_lag_83h', 'elec_prices_lag_84h', 'elec_prices_lag_85h', 'elec_prices_lag_86h', 'elec_prices_lag_87h', 'elec_prices_lag_88h', 'elec_prices_lag_89h', 'elec_prices_lag_90h', 'elec_prices_lag_91h', 'elec_prices_lag_92h', 'elec_prices_lag_93h', 'elec_prices_lag_94h', 'elec_prices_lag_95h', 'elec_prices_lag_96h', 'elec_prices_lag_97h', 'elec_prices_lag_98h', 'elec_prices_lag_99h', 'day_of_week', 'day_of_year', 'week_of_year', 'month']</t>
+          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>['elec_prices', 't+1', 't+2', 't+3', 't+4', 't+5', 't+6', 't+7', 't+8', 't+9', 't+10', 't+11', 't+12', 't+13', 't+14', 't+15', 't+16', 't+17', 't+18', 't+19', 't+20', 't+21', 't+22', 't+23']</t>
+          <t>2019-01-01</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2020-01-01</t>
+          <t>2020-10-18</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2020-12-31</t>
+          <t>2020-09-18</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>2020-03-01</t>
+          <t>2020-12-30</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>2020-04-30</t>
+          <t>[1, 100]</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>[1, 100]</t>
-        </is>
-      </c>
-      <c r="P13" t="inlineStr">
-        <is>
           <t>[1, 24]</t>
         </is>
       </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>109.2341842651367</v>
       </c>
       <c r="R13" t="n">
-        <v>50.47422766685486</v>
+        <v>7.160350740010667</v>
+      </c>
+      <c r="S13" t="n">
+        <v>7.661068111841748</v>
+      </c>
+      <c r="T13" t="n">
+        <v>8.488496558771201</v>
+      </c>
+      <c r="U13" t="n">
+        <v>9.058127973125861</v>
+      </c>
+      <c r="V13" t="n">
+        <v>9.716995557884346</v>
+      </c>
+      <c r="W13" t="n">
+        <v>11.00071884602135</v>
+      </c>
+      <c r="X13" t="n">
+        <v>12.21250512508228</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>12.8957019764395</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>14.45828429381735</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>15.71019571229765</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>15.89446680720623</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>16.14476038209878</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>16.80836881524241</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>16.8217579001212</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>14.50119619954854</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>13.5512524678229</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>15.28367463440186</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>19.26874810967119</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>26.72486902667482</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>24.81549827150404</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>17.20429074214979</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>12.45228680381365</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>9.583450519777916</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>10.19072392265938</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0.6026170294333777</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0.5490378956459447</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0.4603324782675918</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0.3762578792806599</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0.3037837207385077</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>0.1810481200992958</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>0.08978250579155855</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>0.09094564654956594</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>0.01859847261875835</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>-0.02761193244704518</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>-0.05195998145239478</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>-0.1427778170371257</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>-0.2485846205592053</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>-0.1909978739965343</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>-0.1058889244316192</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>-0.08954622515206245</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>-0.2813285585250849</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>-0.2831817775469818</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>-0.1959723592488951</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>-0.270511185115818</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>-0.2570325966740374</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>-0.1519347662477679</v>
+      </c>
+      <c r="BL13" t="n">
+        <v>0.1156333546064622</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>-0.1087980021616228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>